<commit_message>
Updates for report by xl
</commit_message>
<xml_diff>
--- a/code/experiment151207.xlsx
+++ b/code/experiment151207.xlsx
@@ -1,15 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26505"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fxleos/Documents/MATLAB/EV_Grid/code/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="14240" yWindow="1800" windowWidth="14800" windowHeight="8020"/>
   </bookViews>
   <sheets>
     <sheet name="151130" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -46,51 +56,63 @@
     <t>Car</t>
   </si>
   <si>
-    <t>[0,4,4,4]</t>
-  </si>
-  <si>
-    <t>[0,7,7,7]</t>
-  </si>
-  <si>
-    <t>[0,1,4,7]</t>
-  </si>
-  <si>
-    <t>151130_1k_1k_0111</t>
-  </si>
-  <si>
-    <t>151130_1k_1k_0444</t>
-  </si>
-  <si>
-    <t>151130_1k_1k_0777</t>
-  </si>
-  <si>
-    <t>151130_1k_1k_0147</t>
-  </si>
-  <si>
-    <t>151130_1k_50_0147</t>
-  </si>
-  <si>
-    <t>151130_1k_100_0147</t>
-  </si>
-  <si>
-    <t>151130_1k_300_0147</t>
-  </si>
-  <si>
-    <t>151130_1k_500_0147</t>
-  </si>
-  <si>
     <t>cost minimization</t>
+  </si>
+  <si>
+    <t>[0,3,3,3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0,5,5,5]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0,1,3,5]</t>
+  </si>
+  <si>
+    <t>151207_1k_1k_0111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>151207_1k_1k_0333</t>
+  </si>
+  <si>
+    <t>151207_1k_1k_0555</t>
+  </si>
+  <si>
+    <t>151207_1k_1k_0135</t>
+  </si>
+  <si>
+    <t>151207_1k_200_0135</t>
+  </si>
+  <si>
+    <t>151207_1k_400_0135</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>151207_1k_600_0135</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>151207_1k_800_0135</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -177,12 +199,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="DengXian Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -212,12 +234,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="DengXian" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -423,19 +445,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="3" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="3" width="14.83203125" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -458,15 +480,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -481,168 +503,168 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4">
+        <v>1000</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>1000</v>
+      </c>
+      <c r="C5">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>1000</v>
-      </c>
-      <c r="C4">
-        <v>1000</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5">
-        <v>1000</v>
-      </c>
-      <c r="C5">
-        <v>1000</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" t="s">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6">
+        <v>200</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>1000</v>
+      </c>
+      <c r="C7">
+        <v>400</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>1000</v>
+      </c>
+      <c r="C8">
+        <v>600</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>1000</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
-        <v>1000</v>
-      </c>
-      <c r="C7">
-        <v>100</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8">
-        <v>1000</v>
-      </c>
-      <c r="C8">
-        <v>300</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
       <c r="B9">
         <v>1000</v>
       </c>
       <c r="C9">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -654,10 +676,11 @@
         <v>4</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>